<commit_message>
Added the converter for the bioscreen
</commit_message>
<xml_diff>
--- a/template_platereader.xlsx
+++ b/template_platereader.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upct-my.sharepoint.com/personal/alberto_garre_upct_es/Documents/MariaZambrano_UPCT-UCO/03_coding/biogrowth4/biogrowth4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_AD4D2F04E46CFB4ACB3E20DEB556E566683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC650B33-66D3-488C-9DAE-56F6B4DBFCF0}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_AD4D2F04E46CFB4ACB3E20DEB556E566683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F336D3F6-7856-4C7D-BA51-787B2832940F}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>condition</t>
   </si>
@@ -80,15 +79,6 @@
   </si>
   <si>
     <t>Blank</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>direction</t>
-  </si>
-  <si>
-    <t>last</t>
   </si>
 </sst>
 </file>
@@ -421,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -581,43 +571,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A30B8B-4E1A-422E-8D52-1E4BC12BF049}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>